<commit_message>
Bilder von den Konzepten
</commit_message>
<xml_diff>
--- a/Stundenerfassung/Stundenerfassung.xlsx
+++ b/Stundenerfassung/Stundenerfassung.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="24918" windowHeight="11820" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="24918" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Stundenerfassung" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
   <si>
     <t>Thema</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Testinformationen in SoftwareVersionsDatabase geschrieben</t>
+  </si>
+  <si>
+    <t>Erstellung Skizzen</t>
   </si>
 </sst>
 </file>
@@ -522,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -887,6 +890,34 @@
       </c>
       <c r="D25">
         <v>2.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="3">
+        <v>42890</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="3">
+        <v>42890</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -979,7 +1010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Grundgerüst der ETIC2 Applikation erstellt
</commit_message>
<xml_diff>
--- a/Stundenerfassung/Stundenerfassung.xlsx
+++ b/Stundenerfassung/Stundenerfassung.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
   <si>
     <t>Thema</t>
   </si>
@@ -525,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -911,13 +911,27 @@
         <v>42890</v>
       </c>
       <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
         <v>10</v>
-      </c>
-      <c r="C27" t="s">
-        <v>26</v>
       </c>
       <c r="D27">
         <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="3">
+        <v>42891</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -931,7 +945,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Neue Version der Dokumentation hinzugefügt
</commit_message>
<xml_diff>
--- a/Stundenerfassung/Stundenerfassung.xlsx
+++ b/Stundenerfassung/Stundenerfassung.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="24918" windowHeight="11406"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="24918" windowHeight="11406" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Stundenerfassung" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="69">
   <si>
     <t>Thema</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>offen</t>
+  </si>
+  <si>
+    <t>17.07.2017-23.07.2017</t>
   </si>
 </sst>
 </file>
@@ -641,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D75" sqref="D70:D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1684,6 +1687,34 @@
         <v>4</v>
       </c>
     </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="3">
+        <v>42931</v>
+      </c>
+      <c r="B74" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" t="s">
+        <v>59</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="3">
+        <v>42932</v>
+      </c>
+      <c r="B75" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" t="s">
+        <v>59</v>
+      </c>
+      <c r="D75">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1694,8 +1725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1904,10 +1935,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2044,6 +2075,17 @@
       <c r="B12" s="9" t="s">
         <v>62</v>
       </c>
+      <c r="C12">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Skript für Datenbank im MasterDetail Beispiel hinzugefügt
</commit_message>
<xml_diff>
--- a/Stundenerfassung/Stundenerfassung.xlsx
+++ b/Stundenerfassung/Stundenerfassung.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="24918" windowHeight="11406" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="24918" windowHeight="11406"/>
   </bookViews>
   <sheets>
     <sheet name="Stundenerfassung" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="71">
   <si>
     <t>Thema</t>
   </si>
@@ -650,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="D92" sqref="D84:D92"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1957,6 +1957,20 @@
       </c>
       <c r="D92">
         <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="3">
+        <v>42947</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2181,7 +2195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Konzept + Stunden angepasst
</commit_message>
<xml_diff>
--- a/Stundenerfassung/Stundenerfassung.xlsx
+++ b/Stundenerfassung/Stundenerfassung.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="71">
   <si>
     <t>Thema</t>
   </si>
@@ -650,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2015,6 +2015,20 @@
         <v>4</v>
       </c>
     </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="3">
+        <v>42952</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C97" t="s">
+        <v>9</v>
+      </c>
+      <c r="D97">
+        <v>3.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2026,7 +2040,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Refresh Button um View und Database Context zu aktuallisieren
</commit_message>
<xml_diff>
--- a/Stundenerfassung/Stundenerfassung.xlsx
+++ b/Stundenerfassung/Stundenerfassung.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="72">
   <si>
     <t>Thema</t>
   </si>
@@ -653,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2128,6 +2128,34 @@
       </c>
       <c r="D104">
         <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" s="3">
+        <v>42959</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C105" t="s">
+        <v>8</v>
+      </c>
+      <c r="D105">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" s="3">
+        <v>42959</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C106" t="s">
+        <v>10</v>
+      </c>
+      <c r="D106">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WorkspaceView Umschaltung unterschiedliche Ansicht der Daten
Namen geändert und Prinzipt implementiert
</commit_message>
<xml_diff>
--- a/Stundenerfassung/Stundenerfassung.xlsx
+++ b/Stundenerfassung/Stundenerfassung.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="24918" windowHeight="11406" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="24918" windowHeight="11406"/>
   </bookViews>
   <sheets>
     <sheet name="Stundenerfassung" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="73">
   <si>
     <t>Thema</t>
   </si>
@@ -656,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100:D107"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2173,6 +2173,34 @@
       </c>
       <c r="D107">
         <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" s="3">
+        <v>42961</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C108" t="s">
+        <v>8</v>
+      </c>
+      <c r="D108">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" s="3">
+        <v>42962</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C109" t="s">
+        <v>8</v>
+      </c>
+      <c r="D109">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2397,7 +2425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Neues Beispiel zur Navigation von Views
</commit_message>
<xml_diff>
--- a/Stundenerfassung/Stundenerfassung.xlsx
+++ b/Stundenerfassung/Stundenerfassung.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="73">
   <si>
     <t>Thema</t>
   </si>
@@ -656,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2200,6 +2200,20 @@
         <v>8</v>
       </c>
       <c r="D109">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" s="3">
+        <v>42963</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C110" t="s">
+        <v>8</v>
+      </c>
+      <c r="D110">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Abgabeordner erstellt + Stunden angepasst
</commit_message>
<xml_diff>
--- a/Stundenerfassung/Stundenerfassung.xlsx
+++ b/Stundenerfassung/Stundenerfassung.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="24918" windowHeight="11406"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="24918" windowHeight="11406" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stundenerfassung" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="73">
   <si>
     <t>Thema</t>
   </si>
@@ -656,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2259,6 +2259,20 @@
         <v>7</v>
       </c>
     </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" s="3">
+        <v>42967</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C114" t="s">
+        <v>9</v>
+      </c>
+      <c r="D114">
+        <v>3.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2269,8 +2283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2423,7 +2437,7 @@
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2431,7 +2445,7 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2439,7 +2453,7 @@
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2447,7 +2461,7 @@
         <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Refresh nicht neue Datenbankverbindung erstellt + PDF Ausnahmen abgefangen
</commit_message>
<xml_diff>
--- a/Stundenerfassung/Stundenerfassung.xlsx
+++ b/Stundenerfassung/Stundenerfassung.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="24918" windowHeight="11406" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="24918" windowHeight="11406"/>
   </bookViews>
   <sheets>
     <sheet name="Stundenerfassung" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="75">
   <si>
     <t>Thema</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>14.08.2017-20.08.2017</t>
+  </si>
+  <si>
+    <t>Abgabe</t>
+  </si>
+  <si>
+    <t>Diverses</t>
   </si>
 </sst>
 </file>
@@ -656,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2273,6 +2279,34 @@
         <v>3.5</v>
       </c>
     </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" s="3">
+        <v>42968</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C115" t="s">
+        <v>9</v>
+      </c>
+      <c r="D115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" s="3">
+        <v>42968</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C116" t="s">
+        <v>74</v>
+      </c>
+      <c r="D116">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2283,8 +2317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Dokument Aufbau für Gliederung hinzugefügt
</commit_message>
<xml_diff>
--- a/Stundenerfassung/Stundenerfassung.xlsx
+++ b/Stundenerfassung/Stundenerfassung.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="68">
   <si>
     <t>Thema</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Abbruch, da nicht so schnell realisierbar</t>
   </si>
   <si>
-    <t>Kapitel Grundlagen, Zielsetzung, Anfang Methodik beschrieben</t>
-  </si>
-  <si>
     <t xml:space="preserve">Woche </t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>Skripts ausgeführt</t>
   </si>
   <si>
-    <t>Kapitel Methodik, Beschreibung Arbeit beschrieben</t>
-  </si>
-  <si>
     <t>Erstellung Konzept</t>
   </si>
   <si>
@@ -95,12 +89,6 @@
     <t>Skript geschrieben, Firmware Database</t>
   </si>
   <si>
-    <t>Erstellung Skizzen</t>
-  </si>
-  <si>
-    <t>Dokumentation Grundlagen</t>
-  </si>
-  <si>
     <t xml:space="preserve">TestUpdateFirmware </t>
   </si>
   <si>
@@ -116,9 +104,6 @@
     <t>Abspeicherung der Testresultate</t>
   </si>
   <si>
-    <t>Dokumentation Grundlagen, Zielsetzung</t>
-  </si>
-  <si>
     <t>Bemerkungen</t>
   </si>
   <si>
@@ -195,12 +180,6 @@
   </si>
   <si>
     <t>Dokumentation</t>
-  </si>
-  <si>
-    <t>Dokumentation Zielsetzung</t>
-  </si>
-  <si>
-    <t>Dokumentation Beschreibung der Arbeit</t>
   </si>
   <si>
     <t>26.06.2017-02.07.2017</t>
@@ -662,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="E115" sqref="E115"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -690,7 +669,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -712,10 +691,10 @@
         <v>42857</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -726,10 +705,10 @@
         <v>42858</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -740,10 +719,10 @@
         <v>42859</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -754,10 +733,10 @@
         <v>42860</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -767,11 +746,11 @@
       <c r="A7" s="3">
         <v>42862</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
+      <c r="B7" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -782,10 +761,10 @@
         <v>42862</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -796,7 +775,7 @@
         <v>42863</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -813,10 +792,10 @@
         <v>42864</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -827,10 +806,10 @@
         <v>42872</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -841,10 +820,10 @@
         <v>42872</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -855,10 +834,10 @@
         <v>42873</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -869,10 +848,10 @@
         <v>42873</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -883,7 +862,7 @@
         <v>42873</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -896,11 +875,11 @@
       <c r="A16" s="3">
         <v>42876</v>
       </c>
-      <c r="B16" t="s">
-        <v>3</v>
+      <c r="B16" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D16">
         <v>6</v>
@@ -911,10 +890,10 @@
         <v>42877</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -925,10 +904,10 @@
         <v>42878</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D18">
         <v>8</v>
@@ -939,10 +918,10 @@
         <v>42879</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D19">
         <v>8</v>
@@ -952,11 +931,11 @@
       <c r="A20" s="3">
         <v>42880</v>
       </c>
-      <c r="B20" t="s">
-        <v>3</v>
+      <c r="B20" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="D20">
         <v>3.5</v>
@@ -970,7 +949,7 @@
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D21">
         <v>2.5</v>
@@ -984,7 +963,7 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -998,7 +977,7 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -1009,10 +988,10 @@
         <v>42884</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D24">
         <v>2</v>
@@ -1023,10 +1002,10 @@
         <v>42885</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -1037,10 +1016,10 @@
         <v>42886</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D26">
         <v>2.5</v>
@@ -1050,11 +1029,11 @@
       <c r="A27" s="3">
         <v>42890</v>
       </c>
-      <c r="B27" t="s">
-        <v>3</v>
+      <c r="B27" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -1093,7 +1072,7 @@
         <v>42894</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
         <v>13</v>
@@ -1106,11 +1085,11 @@
       <c r="A31" s="3">
         <v>42894</v>
       </c>
-      <c r="B31" t="s">
-        <v>3</v>
+      <c r="B31" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="D31">
         <v>1.5</v>
@@ -1120,11 +1099,11 @@
       <c r="A32" s="3">
         <v>42895</v>
       </c>
-      <c r="B32" t="s">
-        <v>3</v>
+      <c r="B32" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1135,10 +1114,10 @@
         <v>42896</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1148,11 +1127,11 @@
       <c r="A34" s="3">
         <v>42897</v>
       </c>
-      <c r="B34" t="s">
-        <v>3</v>
+      <c r="B34" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -1162,11 +1141,11 @@
       <c r="A35" s="3">
         <v>42897</v>
       </c>
-      <c r="B35" t="s">
-        <v>3</v>
+      <c r="B35" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D35">
         <v>2</v>
@@ -1177,7 +1156,7 @@
         <v>42898</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
         <v>13</v>
@@ -1190,11 +1169,11 @@
       <c r="A37" s="3">
         <v>42898</v>
       </c>
-      <c r="B37" t="s">
-        <v>3</v>
+      <c r="B37" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C37" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1204,11 +1183,11 @@
       <c r="A38" s="3">
         <v>42900</v>
       </c>
-      <c r="B38" t="s">
-        <v>3</v>
+      <c r="B38" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C38" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="D38">
         <v>4</v>
@@ -1219,7 +1198,7 @@
         <v>42901</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C39" t="s">
         <v>13</v>
@@ -1234,10 +1213,10 @@
         <v>42901</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D40">
         <v>4</v>
@@ -1248,10 +1227,10 @@
         <v>42902</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D41">
         <v>4</v>
@@ -1262,10 +1241,10 @@
         <v>42902</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D42">
         <v>4</v>
@@ -1276,10 +1255,10 @@
         <v>42903</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C43" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D43">
         <v>5</v>
@@ -1290,10 +1269,10 @@
         <v>42903</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D44">
         <v>2</v>
@@ -1303,11 +1282,11 @@
       <c r="A45" s="3">
         <v>42904</v>
       </c>
-      <c r="B45" t="s">
-        <v>3</v>
+      <c r="B45" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C45" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D45">
         <v>6</v>
@@ -1318,10 +1297,10 @@
         <v>42905</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C46" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D46">
         <v>6</v>
@@ -1332,10 +1311,10 @@
         <v>42906</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C47" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -1346,10 +1325,10 @@
         <v>42906</v>
       </c>
       <c r="B48" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C48" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D48">
         <v>4</v>
@@ -1360,10 +1339,10 @@
         <v>42907</v>
       </c>
       <c r="B49" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D49">
         <v>2</v>
@@ -1374,7 +1353,7 @@
         <v>42908</v>
       </c>
       <c r="B50" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C50" t="s">
         <v>13</v>
@@ -1388,10 +1367,10 @@
         <v>42909</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C51" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D51">
         <v>6</v>
@@ -1401,11 +1380,11 @@
       <c r="A52" s="3">
         <v>42909</v>
       </c>
-      <c r="B52" t="s">
-        <v>3</v>
+      <c r="B52" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C52" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -1416,10 +1395,10 @@
         <v>42910</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C53" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D53">
         <v>4</v>
@@ -1429,11 +1408,11 @@
       <c r="A54" s="3">
         <v>42911</v>
       </c>
-      <c r="B54" t="s">
-        <v>3</v>
+      <c r="B54" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="D54">
         <v>6</v>
@@ -1444,10 +1423,10 @@
         <v>42912</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C55" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D55">
         <v>4</v>
@@ -1458,10 +1437,10 @@
         <v>42913</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C56" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D56">
         <v>4</v>
@@ -1472,10 +1451,10 @@
         <v>42914</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C57" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D57">
         <v>4</v>
@@ -1486,10 +1465,10 @@
         <v>42915</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C58" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D58">
         <v>2</v>
@@ -1500,10 +1479,10 @@
         <v>42916</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C59" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D59">
         <v>2</v>
@@ -1514,10 +1493,10 @@
         <v>42917</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C60" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D60">
         <v>2</v>
@@ -1527,11 +1506,11 @@
       <c r="A61" s="3">
         <v>42918</v>
       </c>
-      <c r="B61" t="s">
-        <v>3</v>
+      <c r="B61" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C61" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -1542,10 +1521,10 @@
         <v>42919</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C62" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D62">
         <v>4.5</v>
@@ -1556,7 +1535,7 @@
         <v>42919</v>
       </c>
       <c r="B63" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C63" t="s">
         <v>13</v>
@@ -1570,10 +1549,10 @@
         <v>42920</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C64" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D64">
         <v>7</v>
@@ -1584,10 +1563,10 @@
         <v>42921</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C65" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D65">
         <v>7</v>
@@ -1598,10 +1577,10 @@
         <v>42922</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C66" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D66">
         <v>5</v>
@@ -1612,10 +1591,10 @@
         <v>42923</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C67" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D67">
         <v>5</v>
@@ -1626,10 +1605,10 @@
         <v>42924</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C68" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D68">
         <v>3.5</v>
@@ -1639,11 +1618,11 @@
       <c r="A69" s="3">
         <v>42925</v>
       </c>
-      <c r="B69" t="s">
-        <v>3</v>
+      <c r="B69" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C69" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="D69">
         <v>4</v>
@@ -1654,10 +1633,10 @@
         <v>42928</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C70" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D70">
         <v>4</v>
@@ -1668,10 +1647,10 @@
         <v>42929</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C71" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D71">
         <v>4</v>
@@ -1682,10 +1661,10 @@
         <v>42930</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C72" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D72">
         <v>5</v>
@@ -1696,10 +1675,10 @@
         <v>42931</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C73" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D73">
         <v>4</v>
@@ -1709,11 +1688,11 @@
       <c r="A74" s="3">
         <v>42931</v>
       </c>
-      <c r="B74" t="s">
-        <v>3</v>
+      <c r="B74" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C74" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="D74">
         <v>2</v>
@@ -1723,11 +1702,11 @@
       <c r="A75" s="3">
         <v>42932</v>
       </c>
-      <c r="B75" t="s">
-        <v>3</v>
+      <c r="B75" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C75" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="D75">
         <v>4</v>
@@ -1738,10 +1717,10 @@
         <v>42934</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C76" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D76">
         <v>3</v>
@@ -1752,10 +1731,10 @@
         <v>42935</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C77" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D77">
         <v>3</v>
@@ -1765,11 +1744,11 @@
       <c r="A78" s="3">
         <v>42936</v>
       </c>
-      <c r="B78" t="s">
-        <v>3</v>
+      <c r="B78" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C78" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -1780,7 +1759,7 @@
         <v>42937</v>
       </c>
       <c r="B79" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C79" t="s">
         <v>13</v>
@@ -1794,10 +1773,10 @@
         <v>42937</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C80" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D80">
         <v>6</v>
@@ -1808,10 +1787,10 @@
         <v>42938</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C81" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D81">
         <v>5</v>
@@ -1822,7 +1801,7 @@
         <v>42939</v>
       </c>
       <c r="B82" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C82" t="s">
         <v>13</v>
@@ -1836,10 +1815,10 @@
         <v>42939</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C83" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D83">
         <v>7</v>
@@ -1850,10 +1829,10 @@
         <v>42940</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C84" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D84">
         <v>3</v>
@@ -1864,10 +1843,10 @@
         <v>42941</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C85" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D85">
         <v>4</v>
@@ -1878,10 +1857,10 @@
         <v>42942</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C86" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D86">
         <v>3</v>
@@ -1892,10 +1871,10 @@
         <v>42943</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C87" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D87">
         <v>2</v>
@@ -1906,10 +1885,10 @@
         <v>42944</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C88" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D88">
         <v>2</v>
@@ -1920,10 +1899,10 @@
         <v>42945</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C89" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -1934,10 +1913,10 @@
         <v>42945</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C90" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D90">
         <v>2</v>
@@ -1947,11 +1926,11 @@
       <c r="A91" s="3">
         <v>42946</v>
       </c>
-      <c r="B91" t="s">
-        <v>3</v>
+      <c r="B91" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C91" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -1962,10 +1941,10 @@
         <v>42946</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C92" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D92">
         <v>2</v>
@@ -1976,10 +1955,10 @@
         <v>42947</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C93" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D93">
         <v>5</v>
@@ -1990,10 +1969,10 @@
         <v>42948</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C94" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D94">
         <v>6</v>
@@ -2004,10 +1983,10 @@
         <v>42950</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C95" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D95">
         <v>4</v>
@@ -2018,10 +1997,10 @@
         <v>42951</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C96" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D96">
         <v>4</v>
@@ -2032,7 +2011,7 @@
         <v>42952</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C97" t="s">
         <v>9</v>
@@ -2046,7 +2025,7 @@
         <v>42953</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C98" t="s">
         <v>9</v>
@@ -2060,7 +2039,7 @@
         <v>42953</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C99" t="s">
         <v>10</v>
@@ -2074,7 +2053,7 @@
         <v>42954</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C100" t="s">
         <v>9</v>
@@ -2088,7 +2067,7 @@
         <v>42955</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C101" t="s">
         <v>9</v>
@@ -2102,7 +2081,7 @@
         <v>42956</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C102" t="s">
         <v>9</v>
@@ -2116,10 +2095,10 @@
         <v>42957</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C103" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D103">
         <v>5</v>
@@ -2130,10 +2109,10 @@
         <v>42958</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C104" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D104">
         <v>5</v>
@@ -2144,10 +2123,10 @@
         <v>42959</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C105" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D105">
         <v>5</v>
@@ -2158,7 +2137,7 @@
         <v>42959</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C106" t="s">
         <v>10</v>
@@ -2172,10 +2151,10 @@
         <v>42960</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C107" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D107">
         <v>7</v>
@@ -2186,10 +2165,10 @@
         <v>42961</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C108" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D108">
         <v>5</v>
@@ -2200,10 +2179,10 @@
         <v>42962</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C109" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D109">
         <v>4</v>
@@ -2214,10 +2193,10 @@
         <v>42963</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C110" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D110">
         <v>4</v>
@@ -2228,10 +2207,10 @@
         <v>42964</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C111" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D111">
         <v>4</v>
@@ -2242,10 +2221,10 @@
         <v>42965</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C112" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D112">
         <v>4</v>
@@ -2256,7 +2235,7 @@
         <v>42966</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C113" t="s">
         <v>9</v>
@@ -2270,7 +2249,7 @@
         <v>42967</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C114" t="s">
         <v>9</v>
@@ -2284,7 +2263,7 @@
         <v>42968</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C115" t="s">
         <v>9</v>
@@ -2298,14 +2277,73 @@
         <v>42968</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C116" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D116">
         <v>4</v>
       </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" s="3">
+        <v>42969</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C117" t="s">
+        <v>9</v>
+      </c>
+      <c r="D117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" s="3">
+        <v>42969</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C118" t="s">
+        <v>67</v>
+      </c>
+      <c r="D118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" s="3">
+        <v>42969</v>
+      </c>
+      <c r="B119" t="s">
+        <v>3</v>
+      </c>
+      <c r="C119" t="s">
+        <v>51</v>
+      </c>
+      <c r="D119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" s="3">
+        <v>42970</v>
+      </c>
+      <c r="B120" t="s">
+        <v>3</v>
+      </c>
+      <c r="C120" t="s">
+        <v>51</v>
+      </c>
+      <c r="D120">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2315,10 +2353,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2337,186 +2375,178 @@
         <v>12</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" t="s">
-        <v>64</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="1" t="s">
-        <v>57</v>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B28" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2541,13 +2571,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -2555,7 +2585,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>22.5</v>
@@ -2566,7 +2596,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -2577,7 +2607,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -2588,7 +2618,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C5">
         <v>28</v>
@@ -2599,7 +2629,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <v>20</v>
@@ -2610,7 +2640,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C7">
         <v>12</v>
@@ -2621,7 +2651,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C8">
         <v>31</v>
@@ -2632,7 +2662,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C9">
         <v>31.5</v>
@@ -2643,7 +2673,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -2654,7 +2684,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C11">
         <v>36.5</v>
@@ -2665,7 +2695,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C12">
         <v>23</v>
@@ -2676,7 +2706,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C13">
         <v>26.5</v>
@@ -2687,7 +2717,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C14">
         <v>20</v>
@@ -2698,7 +2728,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C15">
         <v>27.5</v>
@@ -2709,7 +2739,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C16">
         <v>35</v>
@@ -2720,7 +2750,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Disposition in Arbeit eingefügt
</commit_message>
<xml_diff>
--- a/Stundenerfassung/Stundenerfassung.xlsx
+++ b/Stundenerfassung/Stundenerfassung.xlsx
@@ -644,7 +644,7 @@
   <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+      <selection activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2339,7 +2339,7 @@
         <v>51</v>
       </c>
       <c r="D120">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Bis Kapitel 5.2.2 gekommen
</commit_message>
<xml_diff>
--- a/Stundenerfassung/Stundenerfassung.xlsx
+++ b/Stundenerfassung/Stundenerfassung.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="68">
   <si>
     <t>Thema</t>
   </si>
@@ -641,9 +641,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
@@ -2343,7 +2343,32 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121" s="3"/>
+      <c r="A121" s="3">
+        <v>42971</v>
+      </c>
+      <c r="B121" t="s">
+        <v>3</v>
+      </c>
+      <c r="C121" t="s">
+        <v>51</v>
+      </c>
+      <c r="D121">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" s="3">
+        <v>42972</v>
+      </c>
+      <c r="B122" t="s">
+        <v>3</v>
+      </c>
+      <c r="C122" t="s">
+        <v>51</v>
+      </c>
+      <c r="D122">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Dokumentation Kapitel Beschreibung der Arbeit abgeschlossen
</commit_message>
<xml_diff>
--- a/Stundenerfassung/Stundenerfassung.xlsx
+++ b/Stundenerfassung/Stundenerfassung.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="24918" windowHeight="11406" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="24918" windowHeight="11406"/>
   </bookViews>
   <sheets>
     <sheet name="Stundenerfassung" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="68">
   <si>
     <t>Thema</t>
   </si>
@@ -641,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:E126"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115:D124"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E124" sqref="E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2396,6 +2396,34 @@
       </c>
       <c r="D124">
         <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" s="3">
+        <v>42975</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C125" t="s">
+        <v>9</v>
+      </c>
+      <c r="D125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" s="3">
+        <v>42975</v>
+      </c>
+      <c r="B126" t="s">
+        <v>3</v>
+      </c>
+      <c r="C126" t="s">
+        <v>51</v>
+      </c>
+      <c r="D126">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2612,7 +2640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>